<commit_message>
Fix data schema table, fix navbar filenames, add drift exp plots
</commit_message>
<xml_diff>
--- a/md-docs/tables/data schema validation.xlsx
+++ b/md-docs/tables/data schema validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessandrolavelli/mlcube/product/platform/ml3-platform-docs/md-docs/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GiovanniGiacometti\Desktop\MLCube\Repositories\ml3-platform-docs\md-docs\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0706B962-B99B-814D-9703-919A5624DD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2459991-E959-4334-BFE4-948F925B5C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20980" activeTab="1" xr2:uid="{02A6762C-53C8-684C-A163-776858D1F132}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{02A6762C-53C8-684C-A163-776858D1F132}"/>
   </bookViews>
   <sheets>
     <sheet name="qts" sheetId="2" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -192,13 +192,16 @@
   </si>
   <si>
     <t>&gt;=0</t>
+  </si>
+  <si>
+    <t>FLOAT, CATEGORY, STRING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,6 +240,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -343,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -376,9 +387,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -716,25 +728,25 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.69921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="45.83203125" customWidth="1"/>
+    <col min="10" max="10" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -772,7 +784,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -810,7 +822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -848,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -886,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -924,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -962,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1000,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1038,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1076,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1114,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1152,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1190,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1228,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1266,7 +1278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1304,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1342,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
@@ -1380,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1416,7 +1428,7 @@
       </c>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>21</v>
       </c>
@@ -1454,7 +1466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>24</v>
       </c>
@@ -1492,61 +1504,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F25" s="17"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F27" s="17"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F32" s="17"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F36" s="17"/>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F39" s="17"/>
     </row>
   </sheetData>
@@ -1564,25 +1576,25 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.69921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="45.83203125" customWidth="1"/>
+    <col min="10" max="10" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1598,7 +1610,9 @@
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1618,7 +1632,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1634,7 +1648,9 @@
       <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1654,7 +1670,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1670,7 +1686,9 @@
       <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1690,7 +1708,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1706,7 +1724,9 @@
       <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1726,7 +1746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1742,7 +1762,9 @@
       <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1762,7 +1784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1778,7 +1800,9 @@
       <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1798,7 +1822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1814,7 +1838,9 @@
       <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1834,7 +1860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
@@ -1850,7 +1876,9 @@
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1870,7 +1898,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1886,7 +1914,9 @@
       <c r="E9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G9" s="3" t="s">
         <v>20</v>
       </c>
@@ -1906,7 +1936,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1922,7 +1952,9 @@
       <c r="E10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1942,7 +1974,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -1958,7 +1990,9 @@
       <c r="E11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1978,7 +2012,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1994,7 +2028,9 @@
       <c r="E12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G12" s="3" t="s">
         <v>20</v>
       </c>
@@ -2014,7 +2050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -2030,7 +2066,9 @@
       <c r="E13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G13" s="3" t="s">
         <v>20</v>
       </c>
@@ -2050,7 +2088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -2066,7 +2104,9 @@
       <c r="E14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G14" s="3" t="s">
         <v>18</v>
       </c>
@@ -2086,7 +2126,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
@@ -2102,7 +2142,9 @@
       <c r="E15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G15" s="3" t="s">
         <v>18</v>
       </c>
@@ -2122,7 +2164,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -2138,7 +2180,9 @@
       <c r="E16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G16" s="3" t="s">
         <v>18</v>
       </c>
@@ -2158,7 +2202,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -2174,7 +2218,9 @@
       <c r="E17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G17" s="3" t="s">
         <v>18</v>
       </c>
@@ -2194,7 +2240,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -2210,7 +2256,9 @@
       <c r="E18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G18" s="13" t="s">
         <v>23</v>
       </c>
@@ -2230,7 +2278,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>21</v>
       </c>
@@ -2246,7 +2294,9 @@
       <c r="E19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="12"/>
+      <c r="F19" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G19" s="12" t="s">
         <v>22</v>
       </c>
@@ -2266,7 +2316,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>24</v>
       </c>
@@ -2282,7 +2332,9 @@
       <c r="E20" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="12"/>
+      <c r="F20" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="G20" s="12" t="s">
         <v>19</v>
       </c>
@@ -2538,15 +2590,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="779550f5-748f-434c-b3fe-a92f7f37a8b2">
@@ -2555,6 +2598,15 @@
     <TaxCatchAll xmlns="1cb8a36e-27df-4b66-9ffb-80c701d247e0" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2577,14 +2629,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B22CDA34-CF6E-458A-B76C-197711286DE0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34611D96-B228-40BE-A3B4-068F3E2B3087}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2599,4 +2643,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B22CDA34-CF6E-458A-B76C-197711286DE0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>